<commit_message>
H21 Totalmente funcional y validada la importacion de modalidad de Verdadero/Falso
</commit_message>
<xml_diff>
--- a/storage/app/plantillaExcel/ImportarPreguntasTextoCorto.xlsx
+++ b/storage/app/plantillaExcel/ImportarPreguntasTextoCorto.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\SIGEN_Resources\SIGEN\storage\app\plantillaExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F03CB473-F174-46C5-9261-3DE4620C9C3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A998776-6DC6-4391-BA23-AE6A6C832763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{0622C781-A97F-45D9-9ACD-0F1875EEC481}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Preguntas Texto Corto" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,9 +30,53 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
+  <si>
+    <t>Pregunta</t>
+  </si>
+  <si>
+    <t>Opcion</t>
+  </si>
+  <si>
+    <t>Pregunta 1</t>
+  </si>
+  <si>
+    <t>Pregunta 2</t>
+  </si>
+  <si>
+    <t>Pregunta 3</t>
+  </si>
+  <si>
+    <t>Pregunta 4</t>
+  </si>
+  <si>
+    <t>Pregunta 5</t>
+  </si>
+  <si>
+    <t>Opcion 1</t>
+  </si>
+  <si>
+    <t>Opcion 2</t>
+  </si>
+  <si>
+    <t>Opcion 3</t>
+  </si>
+  <si>
+    <t>Opcion 4</t>
+  </si>
+  <si>
+    <t>Opcion 5</t>
+  </si>
+  <si>
+    <t>Opcion 6</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,13 +84,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -61,8 +117,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,12 +434,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82EE6D5-39B6-4ADD-B763-DD534A75A850}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="45.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
H21 Importacion de modalidad de respuesta corta, totalmente funcional
</commit_message>
<xml_diff>
--- a/storage/app/plantillaExcel/ImportarPreguntasTextoCorto.xlsx
+++ b/storage/app/plantillaExcel/ImportarPreguntasTextoCorto.xlsx
@@ -8,7 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\SIGEN_Resources\SIGEN\storage\app\plantillaExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A998776-6DC6-4391-BA23-AE6A6C832763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AF262E-93DD-4D09-AAA9-A92E3FA497F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="MLui3soU//qlUnXwMsS6Y6+SwdxhsgtRV4DH2tr7uMVNi2APzW/QjFjniE+pqbYxk+caUz+BWcysYSSI6S20wQ==" workbookSaltValue="HS2pZ9LC0ZlANDsQRO33nw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{0622C781-A97F-45D9-9ACD-0F1875EEC481}"/>
   </bookViews>
@@ -31,52 +32,112 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
-  <si>
-    <t>Pregunta</t>
-  </si>
-  <si>
-    <t>Opcion</t>
-  </si>
-  <si>
-    <t>Pregunta 1</t>
-  </si>
-  <si>
-    <t>Pregunta 2</t>
-  </si>
-  <si>
-    <t>Pregunta 3</t>
-  </si>
-  <si>
-    <t>Pregunta 4</t>
-  </si>
-  <si>
-    <t>Pregunta 5</t>
-  </si>
-  <si>
-    <t>Opcion 1</t>
-  </si>
-  <si>
-    <t>Opcion 2</t>
-  </si>
-  <si>
-    <t>Opcion 3</t>
-  </si>
-  <si>
-    <t>Opcion 4</t>
-  </si>
-  <si>
-    <t>Opcion 5</t>
-  </si>
-  <si>
-    <t>Opcion 6</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>¿Qué?</t>
+  </si>
+  <si>
+    <t>Preguntas</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NOTA: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Es importante que para agregar una nueva pregunta ubique las preguntas en la fila 5</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> si no se ubica y se deja vacio no se identificara la pregunta y las posibles respuestas no seran almacenadas. Las opciones se listaran seguida de la pregunta. Ver ejemplo.</t>
+    </r>
+  </si>
+  <si>
+    <t>Opciones(listar hacia abajo)</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>SII</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>O si</t>
+  </si>
+  <si>
+    <t>No se</t>
+  </si>
+  <si>
+    <t>no se</t>
+  </si>
+  <si>
+    <t>Nooo seee</t>
+  </si>
+  <si>
+    <t>Ayer</t>
+  </si>
+  <si>
+    <t>aller</t>
+  </si>
+  <si>
+    <t>antes de ahora</t>
+  </si>
+  <si>
+    <t>aier</t>
+  </si>
+  <si>
+    <t>Verificacion de plantilla</t>
+  </si>
+  <si>
+    <t>4TC</t>
+  </si>
+  <si>
+    <t>¿Por qué?</t>
+  </si>
+  <si>
+    <t>¿Cuándo?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,8 +151,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,12 +185,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -113,13 +216,243 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,138 +767,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82EE6D5-39B6-4ADD-B763-DD534A75A850}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="48.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" style="7"/>
+    <col min="3" max="3" width="48.42578125" style="8"/>
+    <col min="4" max="16384" width="48.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" spans="1:15" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
+      <c r="D10" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="QKSGJrvh3BL6DVZQ8UA6MgLIeCnoHkMLwXHAaJ280R9G5QUWgmyo+ErbvNFhD2UtA0BRbeaXKaqiAmxI7cNuFQ==" saltValue="v3H/NpWkh5mpiZEYk8LCWA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D2"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>